<commit_message>
spreadsheet added unemployemtn override
</commit_message>
<xml_diff>
--- a/documentation/COVID-19 Changes/September/LSFIM_KY_v5.xlsx
+++ b/documentation/COVID-19 Changes/September/LSFIM_KY_v5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/malcalakovalski/Documents/GitHub/Fiscal-Impact-Measure/documentation/COVID-19 Changes/September/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EA40B64-1853-AC4B-B6A1-B88B8B6B36C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2E1D3F6-1411-A545-8264-7845C922E84D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-320" yWindow="540" windowWidth="33600" windowHeight="18880" activeTab="2" xr2:uid="{BAFE3F49-3B7E-4387-938E-5F3D7AC6DAFE}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18880" xr2:uid="{BAFE3F49-3B7E-4387-938E-5F3D7AC6DAFE}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -692,7 +692,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -3173,6 +3173,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3194,29 +3209,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="3" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -3709,11 +3709,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{412AAB1A-8B83-4A8D-A21D-8EE870D0279B}">
   <dimension ref="A1:AN95"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="J26" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="I26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="L37" sqref="L37"/>
+      <selection pane="bottomRight" activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11204,68 +11204,68 @@
       <c r="M1" s="46"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A2" s="303" t="s">
+      <c r="A2" s="308" t="s">
         <v>104</v>
       </c>
-      <c r="B2" s="303"/>
-      <c r="C2" s="303"/>
-      <c r="D2" s="303"/>
-      <c r="E2" s="303"/>
-      <c r="F2" s="303"/>
-      <c r="G2" s="303"/>
-      <c r="H2" s="303"/>
-      <c r="I2" s="303"/>
-      <c r="J2" s="303"/>
+      <c r="B2" s="308"/>
+      <c r="C2" s="308"/>
+      <c r="D2" s="308"/>
+      <c r="E2" s="308"/>
+      <c r="F2" s="308"/>
+      <c r="G2" s="308"/>
+      <c r="H2" s="308"/>
+      <c r="I2" s="308"/>
+      <c r="J2" s="308"/>
       <c r="K2" s="77"/>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.2">
-      <c r="A3" s="303" t="s">
+      <c r="A3" s="308" t="s">
         <v>105</v>
       </c>
-      <c r="B3" s="303"/>
-      <c r="C3" s="303"/>
-      <c r="D3" s="303"/>
-      <c r="E3" s="303"/>
-      <c r="F3" s="303"/>
-      <c r="G3" s="303"/>
-      <c r="H3" s="303"/>
-      <c r="I3" s="303"/>
-      <c r="J3" s="303"/>
+      <c r="B3" s="308"/>
+      <c r="C3" s="308"/>
+      <c r="D3" s="308"/>
+      <c r="E3" s="308"/>
+      <c r="F3" s="308"/>
+      <c r="G3" s="308"/>
+      <c r="H3" s="308"/>
+      <c r="I3" s="308"/>
+      <c r="J3" s="308"/>
       <c r="K3" s="77"/>
     </row>
     <row r="4" spans="1:24" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="304"/>
-      <c r="B4" s="304"/>
-      <c r="C4" s="304"/>
-      <c r="D4" s="304"/>
-      <c r="E4" s="304"/>
-      <c r="F4" s="304"/>
-      <c r="G4" s="304"/>
-      <c r="H4" s="304"/>
-      <c r="I4" s="304"/>
-      <c r="J4" s="304"/>
-      <c r="K4" s="309" t="s">
+      <c r="A4" s="309"/>
+      <c r="B4" s="309"/>
+      <c r="C4" s="309"/>
+      <c r="D4" s="309"/>
+      <c r="E4" s="309"/>
+      <c r="F4" s="309"/>
+      <c r="G4" s="309"/>
+      <c r="H4" s="309"/>
+      <c r="I4" s="309"/>
+      <c r="J4" s="309"/>
+      <c r="K4" s="314" t="s">
         <v>161</v>
       </c>
-      <c r="L4" s="309"/>
-      <c r="M4" s="309"/>
-      <c r="N4" s="309"/>
+      <c r="L4" s="314"/>
+      <c r="M4" s="314"/>
+      <c r="N4" s="314"/>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5" s="47"/>
       <c r="B5" s="48"/>
-      <c r="C5" s="305" t="s">
+      <c r="C5" s="310" t="s">
         <v>106</v>
       </c>
-      <c r="D5" s="306"/>
-      <c r="E5" s="306"/>
-      <c r="F5" s="306"/>
-      <c r="G5" s="306"/>
-      <c r="H5" s="306"/>
-      <c r="I5" s="306"/>
-      <c r="J5" s="307"/>
+      <c r="D5" s="311"/>
+      <c r="E5" s="311"/>
+      <c r="F5" s="311"/>
+      <c r="G5" s="311"/>
+      <c r="H5" s="311"/>
+      <c r="I5" s="311"/>
+      <c r="J5" s="312"/>
       <c r="K5" s="78"/>
-      <c r="L5" s="308" t="s">
+      <c r="L5" s="313" t="s">
         <v>107</v>
       </c>
       <c r="M5" s="282"/>
@@ -11276,16 +11276,16 @@
         <v>109</v>
       </c>
       <c r="B6" s="49"/>
-      <c r="C6" s="311">
+      <c r="C6" s="304">
         <v>2020</v>
       </c>
-      <c r="D6" s="312"/>
-      <c r="E6" s="312"/>
-      <c r="F6" s="312"/>
-      <c r="G6" s="312"/>
-      <c r="H6" s="312"/>
-      <c r="I6" s="312"/>
-      <c r="J6" s="313"/>
+      <c r="D6" s="305"/>
+      <c r="E6" s="305"/>
+      <c r="F6" s="305"/>
+      <c r="G6" s="305"/>
+      <c r="H6" s="305"/>
+      <c r="I6" s="305"/>
+      <c r="J6" s="306"/>
       <c r="K6" s="78" t="s">
         <v>135</v>
       </c>
@@ -11756,12 +11756,12 @@
       <c r="H23">
         <v>0</v>
       </c>
-      <c r="K23" s="314" t="s">
+      <c r="K23" s="307" t="s">
         <v>108</v>
       </c>
-      <c r="L23" s="314"/>
-      <c r="M23" s="314"/>
-      <c r="N23" s="314"/>
+      <c r="L23" s="307"/>
+      <c r="M23" s="307"/>
+      <c r="N23" s="307"/>
       <c r="O23" s="35" t="s">
         <v>146</v>
       </c>
@@ -11930,7 +11930,7 @@
       <c r="S27" s="72"/>
     </row>
     <row r="28" spans="3:23" x14ac:dyDescent="0.2">
-      <c r="I28" s="310" t="s">
+      <c r="I28" s="303" t="s">
         <v>260</v>
       </c>
       <c r="J28" s="82" t="s">
@@ -11981,7 +11981,7 @@
       <c r="H29">
         <v>67</v>
       </c>
-      <c r="I29" s="310"/>
+      <c r="I29" s="303"/>
       <c r="J29" s="82" t="s">
         <v>143</v>
       </c>
@@ -12030,7 +12030,7 @@
         <f>H29</f>
         <v>67</v>
       </c>
-      <c r="I30" s="310"/>
+      <c r="I30" s="303"/>
       <c r="J30" s="82" t="s">
         <v>142</v>
       </c>
@@ -12079,7 +12079,7 @@
         <f>24</f>
         <v>24</v>
       </c>
-      <c r="I31" s="310"/>
+      <c r="I31" s="303"/>
       <c r="J31" s="35" t="s">
         <v>140</v>
       </c>
@@ -12141,7 +12141,7 @@
         <f t="shared" si="8"/>
         <v>24</v>
       </c>
-      <c r="I33" s="310" t="s">
+      <c r="I33" s="303" t="s">
         <v>141</v>
       </c>
       <c r="J33" s="85" t="s">
@@ -12189,7 +12189,7 @@
       </c>
     </row>
     <row r="34" spans="3:23" x14ac:dyDescent="0.2">
-      <c r="I34" s="310"/>
+      <c r="I34" s="303"/>
       <c r="J34" t="s">
         <v>261</v>
       </c>
@@ -12368,6 +12368,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="L5:N5"/>
+    <mergeCell ref="K4:N4"/>
     <mergeCell ref="O22:R22"/>
     <mergeCell ref="S22:V22"/>
     <mergeCell ref="I28:I31"/>
@@ -12375,12 +12381,6 @@
     <mergeCell ref="C6:J6"/>
     <mergeCell ref="K23:N23"/>
     <mergeCell ref="K22:N22"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="L5:N5"/>
-    <mergeCell ref="K4:N4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -12488,22 +12488,22 @@
       <c r="B6" s="41"/>
       <c r="C6" s="41"/>
       <c r="D6" s="41"/>
-      <c r="E6" s="318" t="s">
+      <c r="E6" s="316" t="s">
         <v>87</v>
       </c>
-      <c r="F6" s="318"/>
-      <c r="G6" s="318"/>
-      <c r="H6" s="318"/>
-      <c r="I6" s="318"/>
-      <c r="J6" s="318"/>
-      <c r="K6" s="318"/>
-      <c r="L6" s="318"/>
-      <c r="M6" s="318"/>
-      <c r="N6" s="318"/>
-      <c r="O6" s="318"/>
-      <c r="P6" s="318"/>
-      <c r="Q6" s="318"/>
-      <c r="R6" s="318"/>
+      <c r="F6" s="316"/>
+      <c r="G6" s="316"/>
+      <c r="H6" s="316"/>
+      <c r="I6" s="316"/>
+      <c r="J6" s="316"/>
+      <c r="K6" s="316"/>
+      <c r="L6" s="316"/>
+      <c r="M6" s="316"/>
+      <c r="N6" s="316"/>
+      <c r="O6" s="316"/>
+      <c r="P6" s="316"/>
+      <c r="Q6" s="316"/>
+      <c r="R6" s="316"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" s="315" t="s">
@@ -13239,21 +13239,21 @@
       <c r="E27" s="24"/>
       <c r="F27" s="24"/>
       <c r="G27" s="24"/>
-      <c r="H27" s="316" t="s">
+      <c r="H27" s="317" t="s">
         <v>95</v>
       </c>
-      <c r="I27" s="316"/>
-      <c r="J27" s="316"/>
-      <c r="K27" s="316"/>
-      <c r="L27" s="316"/>
-      <c r="M27" s="316"/>
-      <c r="N27" s="316"/>
-      <c r="O27" s="316"/>
-      <c r="P27" s="316"/>
-      <c r="Q27" s="316"/>
-      <c r="R27" s="316"/>
-      <c r="S27" s="316"/>
-      <c r="T27" s="316"/>
+      <c r="I27" s="317"/>
+      <c r="J27" s="317"/>
+      <c r="K27" s="317"/>
+      <c r="L27" s="317"/>
+      <c r="M27" s="317"/>
+      <c r="N27" s="317"/>
+      <c r="O27" s="317"/>
+      <c r="P27" s="317"/>
+      <c r="Q27" s="317"/>
+      <c r="R27" s="317"/>
+      <c r="S27" s="317"/>
+      <c r="T27" s="317"/>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A28" s="24" t="s">
@@ -13569,21 +13569,21 @@
       <c r="C37" s="10"/>
       <c r="D37" s="10"/>
       <c r="E37" s="10"/>
-      <c r="F37" s="317" t="s">
+      <c r="F37" s="318" t="s">
         <v>99</v>
       </c>
-      <c r="G37" s="317"/>
-      <c r="H37" s="317"/>
-      <c r="I37" s="317"/>
-      <c r="J37" s="317"/>
-      <c r="K37" s="317"/>
-      <c r="L37" s="317"/>
-      <c r="M37" s="317"/>
-      <c r="N37" s="317"/>
-      <c r="O37" s="317"/>
-      <c r="P37" s="317"/>
-      <c r="Q37" s="317"/>
-      <c r="R37" s="317"/>
+      <c r="G37" s="318"/>
+      <c r="H37" s="318"/>
+      <c r="I37" s="318"/>
+      <c r="J37" s="318"/>
+      <c r="K37" s="318"/>
+      <c r="L37" s="318"/>
+      <c r="M37" s="318"/>
+      <c r="N37" s="318"/>
+      <c r="O37" s="318"/>
+      <c r="P37" s="318"/>
+      <c r="Q37" s="318"/>
+      <c r="R37" s="318"/>
     </row>
     <row r="38" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="24" t="s">
@@ -13899,21 +13899,21 @@
       <c r="C48" s="10"/>
       <c r="D48" s="10"/>
       <c r="E48" s="10"/>
-      <c r="F48" s="316" t="s">
+      <c r="F48" s="317" t="s">
         <v>101</v>
       </c>
-      <c r="G48" s="316"/>
-      <c r="H48" s="316"/>
-      <c r="I48" s="316"/>
-      <c r="J48" s="316"/>
-      <c r="K48" s="316"/>
-      <c r="L48" s="316"/>
-      <c r="M48" s="316"/>
-      <c r="N48" s="316"/>
-      <c r="O48" s="316"/>
-      <c r="P48" s="316"/>
-      <c r="Q48" s="316"/>
-      <c r="R48" s="316"/>
+      <c r="G48" s="317"/>
+      <c r="H48" s="317"/>
+      <c r="I48" s="317"/>
+      <c r="J48" s="317"/>
+      <c r="K48" s="317"/>
+      <c r="L48" s="317"/>
+      <c r="M48" s="317"/>
+      <c r="N48" s="317"/>
+      <c r="O48" s="317"/>
+      <c r="P48" s="317"/>
+      <c r="Q48" s="317"/>
+      <c r="R48" s="317"/>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A49" s="24" t="s">
@@ -14225,12 +14225,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="E6:R6"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B10:D10"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="H27:T27"/>
     <mergeCell ref="F37:R37"/>
@@ -14239,6 +14233,12 @@
     <mergeCell ref="B20:D20"/>
     <mergeCell ref="B21:D21"/>
     <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="E6:R6"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -22191,7 +22191,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{304CD302-ECA7-4CE9-B89D-A357A53FDBE8}">
   <dimension ref="A1:M23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
@@ -28134,12 +28134,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FA9F3DB0CD4D844B918872BCED9B9CF9" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="61f75d9b13a46a58fd2456a565edcb9c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cac5d118-ba7b-4807-b700-df6f95cfff50" xmlns:ns3="66951ee6-cd93-49c7-9437-e871b2a117d6" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d86870d415110e2c98f3a885b29630d1" ns2:_="" ns3:_="">
     <xsd:import namespace="cac5d118-ba7b-4807-b700-df6f95cfff50"/>
@@ -28356,6 +28350,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12E610D1-229D-4CC6-A1C9-48F28FFDA50F}">
   <ds:schemaRefs>
@@ -28365,23 +28365,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{170E13C6-C717-4C73-9EC5-EE5855C1B9D0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="cac5d118-ba7b-4807-b700-df6f95cfff50"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="66951ee6-cd93-49c7-9437-e871b2a117d6"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2B484070-5C48-4F32-AF92-870650EA512F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -28398,4 +28381,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{170E13C6-C717-4C73-9EC5-EE5855C1B9D0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="cac5d118-ba7b-4807-b700-df6f95cfff50"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="66951ee6-cd93-49c7-9437-e871b2a117d6"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>